<commit_message>
modif admin send and create
</commit_message>
<xml_diff>
--- a/Blockchain/Excel Participants.xlsx
+++ b/Blockchain/Excel Participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spierre\Desktop\Aurexia Git\aurexiaGit.github.io\Blockchain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBEFBFA-7EC9-40A4-BC37-A844270421DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EFAFE0-CEDC-40B6-AE49-E4C65328A407}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="1125" windowWidth="23340" windowHeight="13815" xr2:uid="{10EA973A-6DB1-4015-A15D-2E4CEA2D52E0}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="23340" windowHeight="13815" xr2:uid="{10EA973A-6DB1-4015-A15D-2E4CEA2D52E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="388">
-  <si>
-    <t xml:space="preserve">Name </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
   <si>
     <t>Grade</t>
   </si>
@@ -51,9 +48,6 @@
     <t>Caroline PLUVINAGE</t>
   </si>
   <si>
-    <t>Inès AIT MASOUR</t>
-  </si>
-  <si>
     <t>Léonard BEAINO</t>
   </si>
   <si>
@@ -1195,6 +1189,48 @@
   </si>
   <si>
     <t>Alain De CIDRAC</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Mélissa GUIOVANNA-LABORE</t>
+  </si>
+  <si>
+    <t>Elsa NOEL</t>
+  </si>
+  <si>
+    <t>Manmeet RANA</t>
+  </si>
+  <si>
+    <t>Laure VEZILIER</t>
+  </si>
+  <si>
+    <t>0x663eD84CC6D51794830C7bAeDf1D99F537939De3</t>
+  </si>
+  <si>
+    <t>mistake allow marble grocery flight river tip fork tired digital armed melody</t>
+  </si>
+  <si>
+    <t>0xBafBFf9ac72f4bB6e84Ec816f3701121becb20aE</t>
+  </si>
+  <si>
+    <t>heavy idea person exercise source front pride rhythm surround frequent boost custom</t>
+  </si>
+  <si>
+    <t>0xc9F46549B556491222A80f92C6FBfac105d144Bc</t>
+  </si>
+  <si>
+    <t>unit vacuum donkey sunset code slogan double celery food educate system evidence</t>
+  </si>
+  <si>
+    <t>0x427d8aD66072C8185D640cDC20A1DBc520EAd522</t>
+  </si>
+  <si>
+    <t>exhibit detail shy side security genuine ancient trouble owner kidney person degree</t>
+  </si>
+  <si>
+    <t>Inès AIT MANSOUR</t>
   </si>
 </sst>
 </file>
@@ -1230,12 +1266,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1550,10 +1587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF45C2EC-38F3-411B-B713-A60E38D51971}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,1808 +1603,1864 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>399</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C45">
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C47">
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C49">
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C50">
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C51">
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C52">
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C54">
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C55">
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B56" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C56">
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B57" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C58">
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C60">
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C61">
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C62">
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C63">
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C64">
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C66">
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C67">
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B73" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B77" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B78" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B79" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B80" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C93">
         <v>1</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C94">
         <v>2</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C96">
         <v>2</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C97">
         <v>2</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C98">
         <v>2</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C100">
         <v>2</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C102">
         <v>1</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C103">
         <v>1</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C104">
         <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C108" s="2">
         <v>2</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C109" s="2">
         <v>1</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C110" s="2">
         <v>2</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C111" s="2">
         <v>1</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C112" s="2">
         <v>2</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C113" s="2">
         <v>3</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C114" s="2">
         <v>3</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C115" s="2">
         <v>2</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C116" s="2">
         <v>2</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C117" s="2">
         <v>1</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C118" s="2">
         <v>1</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C119" s="2">
         <v>3</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C120" s="2">
         <v>1</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C121" s="2">
         <v>1</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C122" s="2">
         <v>1</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C123" s="2">
         <v>3</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C124" s="2">
         <v>3</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C125" s="2">
         <v>1</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C126" s="2">
         <v>2</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C127" s="2">
         <v>2</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C128" s="2">
         <v>1</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C129" s="2">
         <v>1</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C130" s="3">
+        <v>1</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C131" s="3">
+        <v>1</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C132" s="3">
+        <v>3</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C133" s="3">
+        <v>1</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>